<commit_message>
gjorde "na" til "NA"
</commit_message>
<xml_diff>
--- a/data til laktatprofil.xlsx
+++ b/data til laktatprofil.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c3fb2a472a4d152/Skrivebord/R/Arbeidskrav 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c3fb2a472a4d152/Skrivebord/R/arbeidskrav2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{962F472D-90B5-4C27-A040-32EE5AEB0503}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{962F472D-90B5-4C27-A040-32EE5AEB0503}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F387BC42-D472-447C-88B0-6FC5CA3D96BA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9C92DF78-4AFF-43BB-8D0C-07AD3BAE7160}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="19200" windowHeight="9840" xr2:uid="{9C92DF78-4AFF-43BB-8D0C-07AD3BAE7160}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>pre</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>watt_4mmol</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -507,19 +507,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
@@ -552,16 +552,16 @@
         <v>10</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="U1" s="7"/>
       <c r="V1" s="2"/>
@@ -613,7 +613,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I2" s="4">
         <v>3.86</v>
@@ -625,19 +625,19 @@
         <v>5.6</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="4">
         <v>126.7</v>
@@ -701,7 +701,7 @@
         <v>2.37</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I3" s="4">
         <v>2.71</v>
@@ -713,31 +713,31 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="U3" s="5"/>
       <c r="V3" s="3"/>
@@ -786,22 +786,22 @@
         <v>183</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I4" s="4">
         <v>1.0900000000000001</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="K4" s="4">
         <v>1.73</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="M4" s="4">
         <v>2.08</v>
@@ -813,19 +813,19 @@
         <v>3.85</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="T4" s="10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="U4" s="5"/>
       <c r="V4" s="3"/>
@@ -874,28 +874,28 @@
         <v>183</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I5" s="4">
         <v>1.1299999999999999</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="K5" s="8">
         <v>1.28</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="M5" s="4">
         <v>1.74</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O5" s="4">
         <v>3.04</v>
@@ -907,13 +907,13 @@
         <v>297</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="U5" s="5"/>
       <c r="V5" s="3"/>
@@ -947,7 +947,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4">
         <v>24</v>
@@ -971,25 +971,25 @@
         <v>5.45</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="Q6" s="4">
         <v>131.80000000000001</v>
@@ -1035,7 +1035,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="4">
         <v>24</v>
@@ -1062,22 +1062,22 @@
         <v>5.04</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="Q7" s="4">
         <v>134.19999999999999</v>
@@ -1098,7 +1098,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4">
         <v>26</v>
@@ -1128,19 +1128,19 @@
         <v>6.15</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="Q8" s="4">
         <v>155.69999999999999</v>
@@ -1161,7 +1161,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4">
         <v>26</v>
@@ -1179,7 +1179,7 @@
         <v>1.93</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I9" s="4">
         <v>2.65</v>
@@ -1191,19 +1191,19 @@
         <v>4.76</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="Q9" s="4">
         <v>166.2</v>
@@ -1255,16 +1255,16 @@
         <v>184</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I10" s="4">
         <v>1.73</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="K10" s="4">
         <v>2.35</v>
@@ -1279,19 +1279,19 @@
         <v>4.4800000000000004</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="Q10" s="4">
         <v>238.9</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="T10" s="4">
         <v>86.8</v>
@@ -1334,16 +1334,16 @@
         <v>184</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I11" s="4">
         <v>2.5</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="K11" s="4">
         <v>3.28</v>
@@ -1355,13 +1355,13 @@
         <v>4.5199999999999996</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="Q11" s="4">
         <v>205</v>
@@ -1413,16 +1413,16 @@
         <v>179</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I12" s="9">
         <v>1.48</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="K12" s="9">
         <v>1.67</v>
@@ -1440,7 +1440,7 @@
         <v>4.62</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="Q12" s="4">
         <v>264.10000000000002</v>
@@ -1492,22 +1492,22 @@
         <v>179</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I13" s="4">
         <v>1.4</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="K13" s="4">
         <v>1.88</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="M13" s="4">
         <v>2.31</v>
@@ -1556,7 +1556,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="4">
         <v>23</v>
@@ -1580,25 +1580,25 @@
         <v>6.15</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="Q14" s="4">
         <v>107.7</v>
@@ -1635,7 +1635,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="4">
         <v>23</v>
@@ -1662,22 +1662,22 @@
         <v>6.59</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="Q15" s="4">
         <v>127.8</v>

</xml_diff>

<commit_message>
Endret "lac" til "lac."
</commit_message>
<xml_diff>
--- a/data til laktatprofil.xlsx
+++ b/data til laktatprofil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c3fb2a472a4d152/Skrivebord/R/arbeidskrav2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{962F472D-90B5-4C27-A040-32EE5AEB0503}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F387BC42-D472-447C-88B0-6FC5CA3D96BA}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{962F472D-90B5-4C27-A040-32EE5AEB0503}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9123B583-DF2B-4241-B658-CF8E47E868E6}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="360" windowWidth="19200" windowHeight="9840" xr2:uid="{9C92DF78-4AFF-43BB-8D0C-07AD3BAE7160}"/>
   </bookViews>
@@ -45,36 +45,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>lac125</t>
-  </si>
-  <si>
-    <t>lac150</t>
-  </si>
-  <si>
-    <t>lac175</t>
-  </si>
-  <si>
-    <t>lac200</t>
-  </si>
-  <si>
-    <t>lac225</t>
-  </si>
-  <si>
-    <t>lac250</t>
-  </si>
-  <si>
-    <t>lac275</t>
-  </si>
-  <si>
-    <t>lac300</t>
-  </si>
-  <si>
-    <t>lac75</t>
-  </si>
-  <si>
-    <t>lac100</t>
-  </si>
-  <si>
     <t>post</t>
   </si>
   <si>
@@ -109,6 +79,36 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>lac.75</t>
+  </si>
+  <si>
+    <t>lac.100</t>
+  </si>
+  <si>
+    <t>lac.125</t>
+  </si>
+  <si>
+    <t>lac.150</t>
+  </si>
+  <si>
+    <t>lac.175</t>
+  </si>
+  <si>
+    <t>lac.200</t>
+  </si>
+  <si>
+    <t>lac.225</t>
+  </si>
+  <si>
+    <t>lac.250</t>
+  </si>
+  <si>
+    <t>lac.275</t>
+  </si>
+  <si>
+    <t>lac.300</t>
   </si>
 </sst>
 </file>
@@ -507,61 +507,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="L1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="U1" s="7"/>
       <c r="V1" s="2"/>
@@ -601,7 +601,7 @@
         <v>23</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E2" s="4">
         <v>76.7</v>
@@ -613,7 +613,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I2" s="4">
         <v>3.86</v>
@@ -625,19 +625,19 @@
         <v>5.6</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="Q2" s="4">
         <v>126.7</v>
@@ -689,7 +689,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E3" s="4">
         <v>76.7</v>
@@ -701,7 +701,7 @@
         <v>2.37</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I3" s="4">
         <v>2.71</v>
@@ -713,31 +713,31 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="U3" s="5"/>
       <c r="V3" s="3"/>
@@ -777,7 +777,7 @@
         <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E4" s="4">
         <v>76.099999999999994</v>
@@ -786,22 +786,22 @@
         <v>183</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I4" s="4">
         <v>1.0900000000000001</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="K4" s="4">
         <v>1.73</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="M4" s="4">
         <v>2.08</v>
@@ -813,19 +813,19 @@
         <v>3.85</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="T4" s="10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="U4" s="5"/>
       <c r="V4" s="3"/>
@@ -865,7 +865,7 @@
         <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E5" s="4">
         <v>76.099999999999994</v>
@@ -874,28 +874,28 @@
         <v>183</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I5" s="4">
         <v>1.1299999999999999</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="K5" s="8">
         <v>1.28</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="M5" s="4">
         <v>1.74</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="O5" s="4">
         <v>3.04</v>
@@ -907,13 +907,13 @@
         <v>297</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="U5" s="5"/>
       <c r="V5" s="3"/>
@@ -947,13 +947,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C6" s="4">
         <v>24</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E6" s="4">
         <v>58.7</v>
@@ -971,25 +971,25 @@
         <v>5.45</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="Q6" s="4">
         <v>131.80000000000001</v>
@@ -1035,13 +1035,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C7" s="4">
         <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E7" s="4">
         <v>58.7</v>
@@ -1062,22 +1062,22 @@
         <v>5.04</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="Q7" s="4">
         <v>134.19999999999999</v>
@@ -1098,13 +1098,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4">
         <v>26</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E8" s="4">
         <v>56.3</v>
@@ -1128,19 +1128,19 @@
         <v>6.15</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="Q8" s="4">
         <v>155.69999999999999</v>
@@ -1161,13 +1161,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C9" s="4">
         <v>26</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E9" s="4">
         <v>56.3</v>
@@ -1179,7 +1179,7 @@
         <v>1.93</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I9" s="4">
         <v>2.65</v>
@@ -1191,19 +1191,19 @@
         <v>4.76</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="Q9" s="4">
         <v>166.2</v>
@@ -1246,7 +1246,7 @@
         <v>26</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E10" s="4">
         <v>72.8</v>
@@ -1255,16 +1255,16 @@
         <v>184</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I10" s="4">
         <v>1.73</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="K10" s="4">
         <v>2.35</v>
@@ -1279,19 +1279,19 @@
         <v>4.4800000000000004</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="Q10" s="4">
         <v>238.9</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="T10" s="4">
         <v>86.8</v>
@@ -1325,7 +1325,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E11" s="4">
         <v>72.900000000000006</v>
@@ -1334,16 +1334,16 @@
         <v>184</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I11" s="4">
         <v>2.5</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="K11" s="4">
         <v>3.28</v>
@@ -1355,13 +1355,13 @@
         <v>4.5199999999999996</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="Q11" s="4">
         <v>205</v>
@@ -1404,7 +1404,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E12" s="4">
         <v>77.2</v>
@@ -1413,16 +1413,16 @@
         <v>179</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I12" s="9">
         <v>1.48</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="K12" s="9">
         <v>1.67</v>
@@ -1440,7 +1440,7 @@
         <v>4.62</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="Q12" s="4">
         <v>264.10000000000002</v>
@@ -1483,7 +1483,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E13" s="4">
         <v>76.7</v>
@@ -1492,22 +1492,22 @@
         <v>179</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I13" s="4">
         <v>1.4</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="K13" s="4">
         <v>1.88</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="M13" s="4">
         <v>2.31</v>
@@ -1556,13 +1556,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C14" s="4">
         <v>23</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E14" s="4">
         <v>52.9</v>
@@ -1580,25 +1580,25 @@
         <v>6.15</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="Q14" s="4">
         <v>107.7</v>
@@ -1635,13 +1635,13 @@
         <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C15" s="4">
         <v>23</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E15" s="4">
         <v>52.8</v>
@@ -1662,22 +1662,22 @@
         <v>6.59</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="Q15" s="4">
         <v>127.8</v>

</xml_diff>